<commit_message>
Adding topics of implementation and some comments to the ontology
</commit_message>
<xml_diff>
--- a/SuMSO/materials for implementation/SuMSO vocabulary.xlsx
+++ b/SuMSO/materials for implementation/SuMSO vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaubb\Desktop\Sustainable-Meat-Systems-Ontology\SuMSO\materials for implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA885642-5DC3-42A5-A6F2-8EBBF7F99746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA168FA-FA4E-4A1D-A5C7-C899203E9EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8FC6B3B4-AE2C-481D-A7A9-F5814CA108D7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="775">
   <si>
     <t>Terms</t>
   </si>
@@ -2359,6 +2359,9 @@
   </si>
   <si>
     <t>FSSMF Pillar (primary pertinence)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population </t>
   </si>
 </sst>
 </file>
@@ -2897,10 +2900,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M772"/>
+  <dimension ref="A1:M773"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9425,6 +9428,14 @@
         <v>61</v>
       </c>
     </row>
+    <row r="773" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A773" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="B773" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H772">
     <sortCondition ref="B750:B772"/>

</xml_diff>

<commit_message>
Revisions of implementation materials
</commit_message>
<xml_diff>
--- a/SuMSO/materials for implementation/SuMSO vocabulary.xlsx
+++ b/SuMSO/materials for implementation/SuMSO vocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaubb\Desktop\Sustainable-Meat-Systems-Ontology\SuMSO\materials for implementation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9EE7E1-EF50-4DFF-8177-4C62780F3776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F1AB93-0E61-446B-B51A-1E914A717D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8FC6B3B4-AE2C-481D-A7A9-F5814CA108D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8FC6B3B4-AE2C-481D-A7A9-F5814CA108D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Table Guidelines" sheetId="4" r:id="rId1"/>
@@ -2103,9 +2103,6 @@
     <t xml:space="preserve">Description </t>
   </si>
   <si>
-    <t xml:space="preserve">This table provides the list of SuMSO terms. Reference for each term to is provided. We corresponded each term to the FSSMF pillar to which it primarily pertains. </t>
-  </si>
-  <si>
     <t xml:space="preserve">The terms highlighted in blue are those currently covered within OWL SuMSO core ontological module. Terms presenting an “*” are those (also) proposed by stakeholders. Terms presenting a “†” are those stakeholders considered the most relevant and on which their contributions and suggestions for revisions mainly focused. Future implementations will incorporate the rest of the vocabulary and further terms into SuMSO. </t>
   </si>
   <si>
@@ -2356,6 +2353,9 @@
   </si>
   <si>
     <t>worker's socio-cultural background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This table provides the list of SuMSO terms. We corresponded each term to the FSSMF pillar to which it primarily pertains. </t>
   </si>
 </sst>
 </file>
@@ -2841,13 +2841,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485B4C25-27EA-41B2-9566-D9A8B8E9B093}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="91.21875" customWidth="1"/>
+    <col min="1" max="1" width="92.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -2857,7 +2857,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -2870,17 +2870,17 @@
     </row>
     <row r="5" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>688</v>
+        <v>772</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
   </sheetData>
@@ -2896,7 +2896,7 @@
   </sheetPr>
   <dimension ref="A1:M762"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A737" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A736" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -2911,7 +2911,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -4140,7 +4140,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="10" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B149" s="7" t="s">
         <v>59</v>
@@ -4204,7 +4204,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="7" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B157" s="7" t="s">
         <v>59</v>
@@ -4693,7 +4693,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="20" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B217" s="7" t="s">
         <v>59</v>
@@ -4701,7 +4701,7 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="20" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B218" s="7" t="s">
         <v>59</v>
@@ -4709,7 +4709,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="20" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B219" s="7" t="s">
         <v>59</v>
@@ -4717,7 +4717,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="20" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B220" s="7" t="s">
         <v>59</v>
@@ -4737,7 +4737,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="20" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B222" s="7" t="s">
         <v>59</v>
@@ -4745,7 +4745,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="20" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B223" s="7" t="s">
         <v>59</v>
@@ -4753,7 +4753,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="20" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B224" s="7" t="s">
         <v>59</v>
@@ -4785,7 +4785,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="20" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B228" s="7" t="s">
         <v>60</v>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="10" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B238" s="7" t="s">
         <v>60</v>
@@ -4878,7 +4878,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="10" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B239" s="7" t="s">
         <v>60</v>
@@ -4937,7 +4937,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" s="10" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B246" s="7" t="s">
         <v>60</v>
@@ -4989,7 +4989,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" s="10" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B252" s="7" t="s">
         <v>60</v>
@@ -5029,7 +5029,7 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" s="10" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B257" s="7" t="s">
         <v>60</v>
@@ -5070,7 +5070,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" s="10" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B262" s="7" t="s">
         <v>60</v>
@@ -5250,7 +5250,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" s="10" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B284" s="7" t="s">
         <v>60</v>
@@ -5258,7 +5258,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" s="10" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B285" s="7" t="s">
         <v>60</v>
@@ -5367,7 +5367,7 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" s="10" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B298" s="7" t="s">
         <v>60</v>
@@ -5462,7 +5462,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" s="10" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B309" s="7" t="s">
         <v>60</v>
@@ -5495,7 +5495,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" s="10" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B313" s="7" t="s">
         <v>60</v>
@@ -5582,7 +5582,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323" s="7" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B323" s="7" t="s">
         <v>60</v>
@@ -5662,7 +5662,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" s="10" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B332" s="7" t="s">
         <v>60</v>
@@ -5812,7 +5812,7 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349" s="10" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B349" s="7" t="s">
         <v>60</v>
@@ -5945,7 +5945,7 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A364" s="10" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B364" s="7" t="s">
         <v>60</v>
@@ -5980,7 +5980,7 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A368" s="10" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B368" s="7" t="s">
         <v>60</v>
@@ -6033,7 +6033,7 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A374" s="10" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B374" s="7" t="s">
         <v>60</v>
@@ -6131,7 +6131,7 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385" s="10" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B385" s="7" t="s">
         <v>60</v>
@@ -6173,7 +6173,7 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A390" s="10" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B390" s="7" t="s">
         <v>60</v>
@@ -6181,7 +6181,7 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A391" s="10" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B391" s="7" t="s">
         <v>60</v>
@@ -6189,7 +6189,7 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A392" s="10" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B392" s="7" t="s">
         <v>60</v>
@@ -6197,7 +6197,7 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393" s="10" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B393" s="7" t="s">
         <v>60</v>
@@ -6205,7 +6205,7 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A394" s="10" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B394" s="7" t="s">
         <v>60</v>
@@ -6213,7 +6213,7 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A395" s="10" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B395" s="7" t="s">
         <v>60</v>
@@ -6221,7 +6221,7 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A396" s="10" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B396" s="7" t="s">
         <v>60</v>
@@ -6229,7 +6229,7 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397" s="10" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B397" s="7" t="s">
         <v>60</v>
@@ -6392,7 +6392,7 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A416" s="3" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B416" s="1" t="s">
         <v>60</v>
@@ -6542,7 +6542,7 @@
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A433" s="10" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B433" s="7" t="s">
         <v>60</v>
@@ -6550,7 +6550,7 @@
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A434" s="10" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B434" s="7" t="s">
         <v>60</v>
@@ -6558,7 +6558,7 @@
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A435" s="10" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B435" s="7" t="s">
         <v>60</v>
@@ -6566,7 +6566,7 @@
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A436" s="10" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B436" s="7" t="s">
         <v>60</v>
@@ -6574,7 +6574,7 @@
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A437" s="10" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B437" s="7" t="s">
         <v>60</v>
@@ -6582,7 +6582,7 @@
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A438" s="10" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B438" s="7" t="s">
         <v>60</v>
@@ -6590,7 +6590,7 @@
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A439" s="10" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B439" s="7" t="s">
         <v>60</v>
@@ -6598,7 +6598,7 @@
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A440" s="10" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B440" s="7" t="s">
         <v>60</v>
@@ -6851,7 +6851,7 @@
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A469" s="10" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B469" s="7" t="s">
         <v>60</v>
@@ -6859,7 +6859,7 @@
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A470" s="10" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B470" s="7" t="s">
         <v>60</v>
@@ -6867,7 +6867,7 @@
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A471" s="10" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B471" s="7" t="s">
         <v>60</v>
@@ -6875,7 +6875,7 @@
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A472" s="10" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B472" s="7" t="s">
         <v>60</v>
@@ -6883,7 +6883,7 @@
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A473" s="10" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B473" s="7" t="s">
         <v>60</v>
@@ -6891,7 +6891,7 @@
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A474" s="10" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B474" s="7" t="s">
         <v>60</v>
@@ -6899,7 +6899,7 @@
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A475" s="10" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B475" s="7" t="s">
         <v>60</v>
@@ -6907,7 +6907,7 @@
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A476" s="10" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B476" s="7" t="s">
         <v>60</v>
@@ -6915,7 +6915,7 @@
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A477" s="10" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B477" s="7" t="s">
         <v>60</v>
@@ -7112,7 +7112,7 @@
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A500" s="10" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B500" s="7" t="s">
         <v>60</v>
@@ -7120,7 +7120,7 @@
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A501" s="10" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B501" s="7" t="s">
         <v>60</v>
@@ -7128,7 +7128,7 @@
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A502" s="10" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B502" s="7" t="s">
         <v>60</v>
@@ -7136,7 +7136,7 @@
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A503" s="10" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B503" s="7" t="s">
         <v>60</v>
@@ -7144,7 +7144,7 @@
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A504" s="10" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B504" s="7" t="s">
         <v>60</v>
@@ -7152,7 +7152,7 @@
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A505" s="10" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B505" s="7" t="s">
         <v>60</v>
@@ -7160,7 +7160,7 @@
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A506" s="10" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B506" s="7" t="s">
         <v>60</v>
@@ -7168,7 +7168,7 @@
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A507" s="10" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B507" s="7" t="s">
         <v>60</v>
@@ -7176,7 +7176,7 @@
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A508" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B508" s="7" t="s">
         <v>60</v>
@@ -7184,7 +7184,7 @@
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A509" s="10" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B509" s="7" t="s">
         <v>60</v>
@@ -7277,7 +7277,7 @@
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A520" s="10" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B520" s="7" t="s">
         <v>60</v>
@@ -7285,7 +7285,7 @@
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A521" s="10" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B521" s="7" t="s">
         <v>60</v>
@@ -7455,7 +7455,7 @@
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A540" s="10" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B540" s="7" t="s">
         <v>60</v>
@@ -7463,7 +7463,7 @@
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A541" s="10" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B541" s="7" t="s">
         <v>60</v>
@@ -7471,7 +7471,7 @@
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A542" s="10" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B542" s="7" t="s">
         <v>60</v>
@@ -7578,7 +7578,7 @@
     </row>
     <row r="554" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A554" s="10" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B554" s="7" t="s">
         <v>60</v>
@@ -7981,7 +7981,7 @@
     </row>
     <row r="600" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A600" s="10" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B600" s="7" t="s">
         <v>60</v>
@@ -7997,7 +7997,7 @@
     </row>
     <row r="602" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A602" s="10" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B602" s="7" t="s">
         <v>60</v>
@@ -8163,7 +8163,7 @@
     </row>
     <row r="621" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A621" s="4" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B621" s="1" t="s">
         <v>60</v>
@@ -8190,7 +8190,7 @@
     </row>
     <row r="624" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A624" s="7" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B624" s="7" t="s">
         <v>60</v>
@@ -8198,7 +8198,7 @@
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A625" s="10" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B625" s="7" t="s">
         <v>60</v>
@@ -8206,7 +8206,7 @@
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A626" s="11" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B626" s="7" t="s">
         <v>60</v>
@@ -8382,7 +8382,7 @@
     </row>
     <row r="646" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A646" s="10" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B646" s="7" t="s">
         <v>60</v>
@@ -8674,7 +8674,7 @@
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A680" s="7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B680" s="7" t="s">
         <v>61</v>
@@ -9224,7 +9224,7 @@
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A748" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B748" s="1" t="s">
         <v>61</v>
@@ -9312,7 +9312,7 @@
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A759" s="20" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B759" s="7" t="s">
         <v>61</v>

</xml_diff>